<commit_message>
milestone1.2 - Alex Hochberg - 3-14-16
</commit_message>
<xml_diff>
--- a/milestone1/Milestone_1_State_Transition_Table.xlsx
+++ b/milestone1/Milestone_1_State_Transition_Table.xlsx
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AR47" sqref="AR47"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AR54" sqref="AR54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -882,7 +882,7 @@
         <v>46</v>
       </c>
       <c r="AS2" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.3">
@@ -1019,7 +1019,7 @@
         <v>80</v>
       </c>
       <c r="AS3" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:45" x14ac:dyDescent="0.3">
@@ -2260,82 +2260,82 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="J13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="K13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="L13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="M13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="N13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="O13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="P13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Q13" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="R13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="S13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="T13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="U13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="V13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="W13" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="X13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Y13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Z13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AA13" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AB13" t="s">
         <v>80</v>
@@ -2386,7 +2386,7 @@
         <v>80</v>
       </c>
       <c r="AR13" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="AS13" t="s">
         <v>80</v>
@@ -3219,82 +3219,82 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="J20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="K20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="L20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="M20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="N20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="O20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="P20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Q20" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="R20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="S20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="T20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="U20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="V20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="W20" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="X20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Y20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Z20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AA20" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AB20" t="s">
         <v>80</v>
@@ -3345,7 +3345,7 @@
         <v>80</v>
       </c>
       <c r="AR20" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="AS20" t="s">
         <v>80</v>
@@ -3630,82 +3630,82 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="F23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="J23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="K23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="L23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="M23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="N23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="O23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="P23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Q23" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="R23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="S23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="T23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="U23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="V23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="W23" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="X23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Y23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Z23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AA23" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AB23" t="s">
         <v>80</v>
@@ -3756,7 +3756,7 @@
         <v>80</v>
       </c>
       <c r="AR23" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="AS23" t="s">
         <v>80</v>
@@ -4315,82 +4315,82 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="D28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="G28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="J28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="K28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="L28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="M28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="N28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="O28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="P28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Q28" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="R28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="S28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="T28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="U28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="V28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="W28" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="X28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Y28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Z28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AA28" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AB28" t="s">
         <v>80</v>
@@ -4441,7 +4441,7 @@
         <v>80</v>
       </c>
       <c r="AR28" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="AS28" t="s">
         <v>80</v>
@@ -5000,82 +5000,82 @@
         <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="F33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="G33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="J33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="K33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="L33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="M33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="N33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="O33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="P33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Q33" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="R33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="S33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="T33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="U33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="V33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="W33" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="X33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Y33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Z33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AA33" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AB33" t="s">
         <v>80</v>
@@ -5126,7 +5126,7 @@
         <v>80</v>
       </c>
       <c r="AR33" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="AS33" t="s">
         <v>80</v>
@@ -5685,82 +5685,82 @@
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="E38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="F38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="G38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="J38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="K38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="L38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="M38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="N38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="O38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="P38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Q38" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="R38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="S38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="T38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="U38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="V38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="W38" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="X38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Y38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Z38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AA38" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AB38" t="s">
         <v>80</v>
@@ -5811,7 +5811,7 @@
         <v>80</v>
       </c>
       <c r="AR38" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="AS38" t="s">
         <v>80</v>
@@ -5822,82 +5822,82 @@
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="E39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="F39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="G39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="J39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="K39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="L39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="M39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="N39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="O39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="P39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Q39" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="R39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="S39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="T39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="U39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="V39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="W39" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="X39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Y39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Z39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AA39" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AB39" t="s">
         <v>80</v>
@@ -5948,7 +5948,7 @@
         <v>80</v>
       </c>
       <c r="AR39" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="AS39" t="s">
         <v>43</v>
@@ -6918,82 +6918,82 @@
         <v>50</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="F47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="G47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="H47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="I47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="J47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="K47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="L47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="M47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="N47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="O47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="P47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Q47" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="R47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="S47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="T47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="U47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="V47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="W47" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="X47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Y47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="Z47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AA47" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="AB47" t="s">
         <v>80</v>
@@ -7044,7 +7044,7 @@
         <v>80</v>
       </c>
       <c r="AR47" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="AS47" t="s">
         <v>80</v>

</xml_diff>